<commit_message>
ControlPanel component now updates Table
</commit_message>
<xml_diff>
--- a/app/src/data/CEPR_MO_IL.xlsx
+++ b/app/src/data/CEPR_MO_IL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="28992" windowHeight="15792" tabRatio="834" activeTab="2"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="28992" windowHeight="15792" tabRatio="834" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="141">
   <si>
     <t>Grocery, Convenience, and Drug Stores</t>
   </si>
@@ -394,6 +394,66 @@
   </si>
   <si>
     <t>Educational, Guidance, and Career Counselors And Advisors</t>
+  </si>
+  <si>
+    <t>Full-time</t>
+  </si>
+  <si>
+    <t>Part-time</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>AAPI</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Some college</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Below poverty line</t>
+  </si>
+  <si>
+    <t>&lt;200% poverty line</t>
+  </si>
+  <si>
+    <t>No health insurance</t>
+  </si>
+  <si>
+    <t>Child in home</t>
+  </si>
+  <si>
+    <t>Senior (age 65+) in home</t>
+  </si>
+  <si>
+    <t>Less than High School</t>
+  </si>
+  <si>
+    <t>Grocery, Convenience, &amp; Drug Stores</t>
+  </si>
+  <si>
+    <t>Childcare &amp; Social Services</t>
+  </si>
+  <si>
+    <t>Trucking, Warehouse, &amp; Postal Service</t>
   </si>
 </sst>
 </file>
@@ -491,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -549,7 +609,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -905,17 +964,17 @@
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="14.4" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:15" ht="55.05" customHeight="1" thickTop="1">
       <c r="A3" s="12"/>
@@ -1816,11 +1875,11 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="14.4" thickBot="1">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
     </row>
     <row r="36" spans="1:11" ht="55.8" thickTop="1">
       <c r="A36" s="9"/>
@@ -2552,7 +2611,7 @@
       <c r="C67" s="6"/>
     </row>
     <row r="69" spans="1:11" ht="14.4" thickBot="1">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="31" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2576,19 +2635,19 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="8"/>
-      <c r="B71" s="33" t="s">
+      <c r="B71" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="33" t="s">
+      <c r="C71" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D71" s="33" t="s">
+      <c r="D71" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E71" s="33" t="s">
+      <c r="E71" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="F71" s="33" t="s">
+      <c r="F71" s="32" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2596,18 +2655,18 @@
       <c r="A72" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="37">
+      <c r="B72" s="36">
         <v>100</v>
       </c>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="F72" s="33"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="F72" s="32"/>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B73" s="34">
+      <c r="B73" s="33">
         <v>18.27</v>
       </c>
       <c r="C73" s="21">
@@ -2627,7 +2686,7 @@
       <c r="A74" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="34">
+      <c r="B74" s="33">
         <v>14.27</v>
       </c>
       <c r="C74" s="21">
@@ -2647,7 +2706,7 @@
       <c r="A75" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B75" s="34">
+      <c r="B75" s="33">
         <v>11.07</v>
       </c>
       <c r="C75" s="21">
@@ -2667,7 +2726,7 @@
       <c r="A76" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="34">
+      <c r="B76" s="33">
         <v>7.01</v>
       </c>
       <c r="C76" s="21">
@@ -2687,7 +2746,7 @@
       <c r="A77" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B77" s="34">
+      <c r="B77" s="33">
         <v>6.53</v>
       </c>
       <c r="C77" s="21">
@@ -2707,7 +2766,7 @@
       <c r="A78" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="34">
+      <c r="B78" s="33">
         <v>4.2300000000000004</v>
       </c>
       <c r="C78" s="21">
@@ -2727,7 +2786,7 @@
       <c r="A79" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B79" s="34">
+      <c r="B79" s="33">
         <v>2.94</v>
       </c>
       <c r="C79" s="21">
@@ -2747,7 +2806,7 @@
       <c r="A80" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="34">
+      <c r="B80" s="33">
         <v>2.7</v>
       </c>
       <c r="C80" s="21">
@@ -2767,7 +2826,7 @@
       <c r="A81" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B81" s="34">
+      <c r="B81" s="33">
         <v>2.61</v>
       </c>
       <c r="C81" s="21">
@@ -2787,7 +2846,7 @@
       <c r="A82" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="34">
+      <c r="B82" s="33">
         <v>2.02</v>
       </c>
       <c r="C82" s="21">
@@ -2807,7 +2866,7 @@
       <c r="A83" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="37">
+      <c r="B83" s="36">
         <v>100</v>
       </c>
       <c r="C83" s="21"/>
@@ -2818,7 +2877,7 @@
       <c r="A84" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B84" s="34">
+      <c r="B84" s="33">
         <v>19.22</v>
       </c>
       <c r="C84" s="21">
@@ -2838,7 +2897,7 @@
       <c r="A85" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B85" s="34">
+      <c r="B85" s="33">
         <v>18.55</v>
       </c>
       <c r="C85" s="21">
@@ -2858,7 +2917,7 @@
       <c r="A86" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B86" s="34">
+      <c r="B86" s="33">
         <v>5.8</v>
       </c>
       <c r="C86" s="21">
@@ -2878,7 +2937,7 @@
       <c r="A87" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B87" s="34">
+      <c r="B87" s="33">
         <v>5.26</v>
       </c>
       <c r="C87" s="21">
@@ -2898,7 +2957,7 @@
       <c r="A88" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B88" s="34">
+      <c r="B88" s="33">
         <v>3.24</v>
       </c>
       <c r="C88" s="21">
@@ -2918,7 +2977,7 @@
       <c r="A89" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B89" s="34">
+      <c r="B89" s="33">
         <v>3.06</v>
       </c>
       <c r="C89" s="21">
@@ -2938,7 +2997,7 @@
       <c r="A90" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B90" s="34">
+      <c r="B90" s="33">
         <v>2.41</v>
       </c>
       <c r="C90" s="21">
@@ -2958,7 +3017,7 @@
       <c r="A91" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B91" s="34">
+      <c r="B91" s="33">
         <v>2.41</v>
       </c>
       <c r="C91" s="21">
@@ -2978,7 +3037,7 @@
       <c r="A92" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B92" s="34">
+      <c r="B92" s="33">
         <v>2.36</v>
       </c>
       <c r="C92" s="21">
@@ -2998,7 +3057,7 @@
       <c r="A93" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B93" s="34">
+      <c r="B93" s="33">
         <v>2.09</v>
       </c>
       <c r="C93" s="21">
@@ -3018,7 +3077,7 @@
       <c r="A94" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="37">
+      <c r="B94" s="36">
         <v>100</v>
       </c>
       <c r="C94" s="21"/>
@@ -3030,7 +3089,7 @@
       <c r="A95" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="34">
+      <c r="B95" s="33">
         <v>42.26</v>
       </c>
       <c r="C95" s="21">
@@ -3050,7 +3109,7 @@
       <c r="A96" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B96" s="34">
+      <c r="B96" s="33">
         <v>10.39</v>
       </c>
       <c r="C96" s="21">
@@ -3070,7 +3129,7 @@
       <c r="A97" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="34">
+      <c r="B97" s="33">
         <v>7.28</v>
       </c>
       <c r="C97" s="21">
@@ -3090,7 +3149,7 @@
       <c r="A98" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B98" s="34">
+      <c r="B98" s="33">
         <v>3.63</v>
       </c>
       <c r="C98" s="21">
@@ -3110,7 +3169,7 @@
       <c r="A99" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="34">
+      <c r="B99" s="33">
         <v>2.96</v>
       </c>
       <c r="C99" s="21">
@@ -3130,7 +3189,7 @@
       <c r="A100" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B100" s="34">
+      <c r="B100" s="33">
         <v>2.62</v>
       </c>
       <c r="C100" s="21">
@@ -3150,7 +3209,7 @@
       <c r="A101" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B101" s="34">
+      <c r="B101" s="33">
         <v>2.09</v>
       </c>
       <c r="C101" s="21">
@@ -3170,7 +3229,7 @@
       <c r="A102" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B102" s="34">
+      <c r="B102" s="33">
         <v>1.83</v>
       </c>
       <c r="C102" s="21">
@@ -3190,7 +3249,7 @@
       <c r="A103" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B103" s="34">
+      <c r="B103" s="33">
         <v>1.8</v>
       </c>
       <c r="C103" s="21">
@@ -3210,7 +3269,7 @@
       <c r="A104" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B104" s="34">
+      <c r="B104" s="33">
         <v>1.49</v>
       </c>
       <c r="C104" s="21">
@@ -3230,7 +3289,7 @@
       <c r="A105" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B105" s="37">
+      <c r="B105" s="36">
         <v>100</v>
       </c>
       <c r="C105" s="21"/>
@@ -3242,7 +3301,7 @@
       <c r="A106" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="34">
+      <c r="B106" s="33">
         <v>44.65</v>
       </c>
       <c r="C106" s="21">
@@ -3262,7 +3321,7 @@
       <c r="A107" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="34">
+      <c r="B107" s="33">
         <v>23.66</v>
       </c>
       <c r="C107" s="21">
@@ -3282,7 +3341,7 @@
       <c r="A108" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="34">
+      <c r="B108" s="33">
         <v>8.94</v>
       </c>
       <c r="C108" s="21">
@@ -3302,7 +3361,7 @@
       <c r="A109" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B109" s="34">
+      <c r="B109" s="33">
         <v>5.17</v>
       </c>
       <c r="C109" s="21">
@@ -3322,7 +3381,7 @@
       <c r="A110" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="34">
+      <c r="B110" s="33">
         <v>2.92</v>
       </c>
       <c r="C110" s="21">
@@ -3342,7 +3401,7 @@
       <c r="A111" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="34">
+      <c r="B111" s="33">
         <v>1.67</v>
       </c>
       <c r="C111" s="21">
@@ -3362,7 +3421,7 @@
       <c r="A112" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="34">
+      <c r="B112" s="33">
         <v>0.98</v>
       </c>
       <c r="C112" s="21">
@@ -3382,7 +3441,7 @@
       <c r="A113" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="34">
+      <c r="B113" s="33">
         <v>0.81</v>
       </c>
       <c r="C113" s="21">
@@ -3402,7 +3461,7 @@
       <c r="A114" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B114" s="34">
+      <c r="B114" s="33">
         <v>0.63</v>
       </c>
       <c r="C114" s="21">
@@ -3422,7 +3481,7 @@
       <c r="A115" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B115" s="34">
+      <c r="B115" s="33">
         <v>0.6</v>
       </c>
       <c r="C115" s="21">
@@ -3442,7 +3501,7 @@
       <c r="A116" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="37">
+      <c r="B116" s="36">
         <v>100</v>
       </c>
       <c r="D116" s="21"/>
@@ -3453,7 +3512,7 @@
       <c r="A117" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B117" s="34">
+      <c r="B117" s="33">
         <v>17.66</v>
       </c>
       <c r="C117" s="21">
@@ -3473,7 +3532,7 @@
       <c r="A118" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B118" s="34">
+      <c r="B118" s="33">
         <v>8.4499999999999993</v>
       </c>
       <c r="C118" s="21">
@@ -3493,7 +3552,7 @@
       <c r="A119" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B119" s="34">
+      <c r="B119" s="33">
         <v>4.99</v>
       </c>
       <c r="C119" s="21">
@@ -3513,7 +3572,7 @@
       <c r="A120" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B120" s="34">
+      <c r="B120" s="33">
         <v>4.67</v>
       </c>
       <c r="C120" s="21">
@@ -3533,7 +3592,7 @@
       <c r="A121" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B121" s="34">
+      <c r="B121" s="33">
         <v>4.46</v>
       </c>
       <c r="C121" s="21">
@@ -3553,7 +3612,7 @@
       <c r="A122" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B122" s="34">
+      <c r="B122" s="33">
         <v>3.7</v>
       </c>
       <c r="C122" s="21">
@@ -3573,7 +3632,7 @@
       <c r="A123" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B123" s="34">
+      <c r="B123" s="33">
         <v>2.9</v>
       </c>
       <c r="C123" s="21">
@@ -3593,7 +3652,7 @@
       <c r="A124" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B124" s="34">
+      <c r="B124" s="33">
         <v>2.66</v>
       </c>
       <c r="C124" s="21">
@@ -3613,7 +3672,7 @@
       <c r="A125" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B125" s="34">
+      <c r="B125" s="33">
         <v>2.41</v>
       </c>
       <c r="C125" s="21">
@@ -3633,7 +3692,7 @@
       <c r="A126" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B126" s="34">
+      <c r="B126" s="33">
         <v>2.29</v>
       </c>
       <c r="C126" s="21">
@@ -3653,7 +3712,7 @@
       <c r="A127" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B127" s="37">
+      <c r="B127" s="36">
         <v>100</v>
       </c>
       <c r="C127" s="21"/>
@@ -3665,7 +3724,7 @@
       <c r="A128" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B128" s="34">
+      <c r="B128" s="33">
         <v>22.8</v>
       </c>
       <c r="C128" s="21">
@@ -3685,7 +3744,7 @@
       <c r="A129" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B129" s="34">
+      <c r="B129" s="33">
         <v>13.87</v>
       </c>
       <c r="C129" s="21">
@@ -3705,7 +3764,7 @@
       <c r="A130" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B130" s="34">
+      <c r="B130" s="33">
         <v>11.62</v>
       </c>
       <c r="C130" s="21">
@@ -3725,7 +3784,7 @@
       <c r="A131" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B131" s="34">
+      <c r="B131" s="33">
         <v>6.63</v>
       </c>
       <c r="C131" s="21">
@@ -3745,7 +3804,7 @@
       <c r="A132" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B132" s="34">
+      <c r="B132" s="33">
         <v>4.3</v>
       </c>
       <c r="C132" s="21">
@@ -3765,7 +3824,7 @@
       <c r="A133" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B133" s="34">
+      <c r="B133" s="33">
         <v>3.18</v>
       </c>
       <c r="C133" s="21">
@@ -3785,7 +3844,7 @@
       <c r="A134" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B134" s="34">
+      <c r="B134" s="33">
         <v>2.63</v>
       </c>
       <c r="C134" s="21">
@@ -3805,7 +3864,7 @@
       <c r="A135" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B135" s="34">
+      <c r="B135" s="33">
         <v>2.29</v>
       </c>
       <c r="C135" s="21">
@@ -3825,7 +3884,7 @@
       <c r="A136" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B136" s="34">
+      <c r="B136" s="33">
         <v>1.61</v>
       </c>
       <c r="C136" s="21">
@@ -3845,7 +3904,7 @@
       <c r="A137" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B137" s="35">
+      <c r="B137" s="34">
         <v>1.56</v>
       </c>
       <c r="C137" s="23">
@@ -3866,8 +3925,8 @@
         <v>18</v>
       </c>
       <c r="C138" s="21"/>
-      <c r="D138" s="36"/>
-      <c r="F138" s="36"/>
+      <c r="D138" s="35"/>
+      <c r="F138" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3884,10 +3943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -3909,13 +3968,13 @@
         <v>21</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>17</v>
@@ -3924,7 +3983,7 @@
         <v>71</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -3963,788 +4022,653 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>23</v>
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="21">
+        <v>47.7</v>
+      </c>
+      <c r="C3" s="21">
+        <v>63.7</v>
+      </c>
+      <c r="D3" s="21">
+        <v>51</v>
+      </c>
+      <c r="E3" s="21">
+        <v>30.8</v>
+      </c>
+      <c r="F3" s="21">
+        <v>22.4</v>
+      </c>
+      <c r="G3" s="21">
+        <v>52.9</v>
+      </c>
+      <c r="H3" s="21">
+        <v>78.3</v>
+      </c>
+      <c r="I3" s="21">
+        <v>86.1</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B4" s="21">
-        <v>47.7</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C4" s="21">
-        <v>63.7</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="D4" s="21">
-        <v>51</v>
+        <v>16.7</v>
       </c>
       <c r="E4" s="21">
-        <v>30.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F4" s="21">
-        <v>22.4</v>
+        <v>22.2</v>
       </c>
       <c r="G4" s="21">
-        <v>52.9</v>
+        <v>47.1</v>
       </c>
       <c r="H4" s="21">
-        <v>78.3</v>
+        <v>16.5</v>
       </c>
       <c r="I4" s="21">
-        <v>86.1</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="21">
+        <v>32.9</v>
+      </c>
+      <c r="C5" s="21">
+        <v>34.5</v>
+      </c>
+      <c r="D5" s="21">
+        <v>27.1</v>
+      </c>
+      <c r="E5" s="21">
+        <v>42</v>
+      </c>
+      <c r="F5" s="21">
+        <v>38.4</v>
+      </c>
+      <c r="G5" s="21">
+        <v>41.2</v>
+      </c>
+      <c r="H5" s="21">
+        <v>35.4</v>
+      </c>
+      <c r="I5" s="21">
+        <v>35.200000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
+      <c r="A6" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B6" s="21">
+        <v>69</v>
+      </c>
+      <c r="C6" s="21">
+        <v>66.5</v>
+      </c>
+      <c r="D6" s="21">
+        <v>62.6</v>
+      </c>
+      <c r="E6" s="21">
+        <v>69.8</v>
+      </c>
+      <c r="F6" s="21">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G6" s="21">
+        <v>59.9</v>
+      </c>
+      <c r="H6" s="21">
+        <v>68.8</v>
+      </c>
+      <c r="I6" s="21">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="21">
+        <v>9.5</v>
+      </c>
+      <c r="C7" s="21">
+        <v>6.8</v>
+      </c>
+      <c r="D7" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="E7" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="F7" s="21">
+        <v>3</v>
+      </c>
+      <c r="G7" s="21">
+        <v>10.7</v>
+      </c>
+      <c r="H7" s="21">
+        <v>6.4</v>
+      </c>
+      <c r="I7" s="21">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="21">
         <v>78.2</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C8" s="21">
         <v>73.900000000000006</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D8" s="21">
         <v>61</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E8" s="21">
         <v>77.2</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F8" s="21">
         <v>91.7</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G8" s="21">
         <v>67.8</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H8" s="21">
         <v>76.900000000000006</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I8" s="21">
         <v>65.7</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="21">
-        <v>21.8</v>
-      </c>
-      <c r="C7" s="21">
-        <v>26.1</v>
-      </c>
-      <c r="D7" s="21">
-        <v>39</v>
-      </c>
-      <c r="E7" s="21">
-        <v>22.8</v>
-      </c>
-      <c r="F7" s="21">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="G7" s="21">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="H7" s="21">
-        <v>23.1</v>
-      </c>
-      <c r="I7" s="21">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>4</v>
-      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="B9" s="21">
-        <v>65.2</v>
+        <v>21.8</v>
       </c>
       <c r="C9" s="21">
-        <v>59.9</v>
+        <v>26.1</v>
       </c>
       <c r="D9" s="21">
-        <v>61.2</v>
+        <v>39</v>
       </c>
       <c r="E9" s="21">
-        <v>50.7</v>
+        <v>22.8</v>
       </c>
       <c r="F9" s="21">
-        <v>61.2</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="G9" s="21">
-        <v>52</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="H9" s="21">
-        <v>61.6</v>
+        <v>23.1</v>
       </c>
       <c r="I9" s="21">
-        <v>53.8</v>
-      </c>
+        <v>34.299999999999997</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B10" s="21">
-        <v>11.9</v>
+        <v>65.2</v>
       </c>
       <c r="C10" s="21">
-        <v>17.899999999999999</v>
+        <v>59.9</v>
       </c>
       <c r="D10" s="21">
-        <v>13.8</v>
+        <v>61.2</v>
       </c>
       <c r="E10" s="21">
-        <v>34.799999999999997</v>
+        <v>50.7</v>
       </c>
       <c r="F10" s="21">
-        <v>18.399999999999999</v>
+        <v>61.2</v>
       </c>
       <c r="G10" s="21">
-        <v>10.1</v>
+        <v>52</v>
       </c>
       <c r="H10" s="21">
-        <v>17.399999999999999</v>
+        <v>61.6</v>
       </c>
       <c r="I10" s="21">
-        <v>25.3</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="B11" s="21">
-        <v>16.2</v>
+        <v>11.9</v>
       </c>
       <c r="C11" s="21">
-        <v>14.3</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D11" s="21">
-        <v>18.100000000000001</v>
+        <v>13.8</v>
       </c>
       <c r="E11" s="21">
-        <v>12.7</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="F11" s="21">
-        <v>17.100000000000001</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="G11" s="21">
-        <v>35.799999999999997</v>
+        <v>10.1</v>
       </c>
       <c r="H11" s="21">
-        <v>10.199999999999999</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="I11" s="21">
-        <v>15.2</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="B12" s="21">
-        <v>6.2</v>
+        <v>16.2</v>
       </c>
       <c r="C12" s="21">
-        <v>7.4</v>
+        <v>14.3</v>
       </c>
       <c r="D12" s="21">
-        <v>6.4</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="E12" s="21">
-        <v>1.4</v>
+        <v>12.7</v>
       </c>
       <c r="F12" s="21">
-        <v>3</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="G12" s="21">
-        <v>1.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="H12" s="21">
-        <v>10.3</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="I12" s="21">
-        <v>5.0999999999999996</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="B13" s="21">
+        <v>6.2</v>
+      </c>
+      <c r="C13" s="21">
+        <v>7.4</v>
+      </c>
+      <c r="D13" s="21">
+        <v>6.4</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1.4</v>
+      </c>
+      <c r="F13" s="21">
+        <v>3</v>
+      </c>
+      <c r="G13" s="21">
+        <v>1.8</v>
+      </c>
+      <c r="H13" s="21">
+        <v>10.3</v>
+      </c>
+      <c r="I13" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="21">
         <v>0.5</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C14" s="21">
         <v>0.5</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D14" s="21">
         <v>0.5</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E14" s="21">
         <v>0.5</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F14" s="21">
         <v>0.3</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G14" s="21">
         <v>0.4</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H14" s="21">
         <v>0.5</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I14" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="21">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="C14" s="21">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="D14" s="21">
-        <v>16.7</v>
-      </c>
-      <c r="E14" s="21">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="F14" s="21">
-        <v>22.2</v>
-      </c>
-      <c r="G14" s="21">
-        <v>47.1</v>
-      </c>
-      <c r="H14" s="21">
-        <v>16.5</v>
-      </c>
-      <c r="I14" s="21">
-        <v>15.5</v>
-      </c>
-    </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>4</v>
+      <c r="A15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="21">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C15" s="21">
+        <v>7.3</v>
+      </c>
+      <c r="D15" s="21">
+        <v>11.6</v>
+      </c>
+      <c r="E15" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="F15" s="21">
+        <v>10.6</v>
+      </c>
+      <c r="G15" s="21">
+        <v>23.7</v>
+      </c>
+      <c r="H15" s="21">
+        <v>3.6</v>
+      </c>
+      <c r="I15" s="21">
+        <v>6.1</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="B16" s="21">
-        <v>8.1999999999999993</v>
+        <v>22.6</v>
       </c>
       <c r="C16" s="21">
-        <v>7.3</v>
+        <v>24.4</v>
       </c>
       <c r="D16" s="21">
-        <v>11.6</v>
+        <v>32.6</v>
       </c>
       <c r="E16" s="21">
-        <v>5.5</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="F16" s="21">
-        <v>10.6</v>
+        <v>40.4</v>
       </c>
       <c r="G16" s="21">
-        <v>23.7</v>
+        <v>41.6</v>
       </c>
       <c r="H16" s="21">
-        <v>3.6</v>
+        <v>15.9</v>
       </c>
       <c r="I16" s="21">
-        <v>6.1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="B17" s="21">
-        <v>22.6</v>
+        <v>31.5</v>
       </c>
       <c r="C17" s="21">
-        <v>24.4</v>
+        <v>36.6</v>
       </c>
       <c r="D17" s="21">
-        <v>32.6</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="E17" s="21">
-        <v>36.299999999999997</v>
+        <v>44.2</v>
       </c>
       <c r="F17" s="21">
-        <v>40.4</v>
+        <v>36</v>
       </c>
       <c r="G17" s="21">
-        <v>41.6</v>
+        <v>23.8</v>
       </c>
       <c r="H17" s="21">
-        <v>15.9</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="I17" s="21">
-        <v>18</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="B18" s="21">
-        <v>31.5</v>
+        <v>23.5</v>
       </c>
       <c r="C18" s="21">
-        <v>36.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="D18" s="21">
-        <v>35.299999999999997</v>
+        <v>15</v>
       </c>
       <c r="E18" s="21">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="F18" s="21">
-        <v>36</v>
+        <v>10.5</v>
       </c>
       <c r="G18" s="21">
-        <v>23.8</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H18" s="21">
-        <v>37.799999999999997</v>
+        <v>24.5</v>
       </c>
       <c r="I18" s="21">
-        <v>36.4</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="B19" s="21">
-        <v>23.5</v>
+        <v>14.1</v>
       </c>
       <c r="C19" s="21">
-        <v>19.600000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="D19" s="21">
-        <v>15</v>
+        <v>5.4</v>
       </c>
       <c r="E19" s="21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F19" s="21">
-        <v>10.5</v>
+        <v>2.5</v>
       </c>
       <c r="G19" s="21">
-        <v>8.6999999999999993</v>
+        <v>2.1</v>
       </c>
       <c r="H19" s="21">
-        <v>24.5</v>
+        <v>18.3</v>
       </c>
       <c r="I19" s="21">
-        <v>25.1</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="B20" s="21">
-        <v>14.1</v>
+        <v>6</v>
       </c>
       <c r="C20" s="21">
-        <v>12.1</v>
+        <v>6.9</v>
       </c>
       <c r="D20" s="21">
-        <v>5.4</v>
+        <v>9.6</v>
       </c>
       <c r="E20" s="21">
-        <v>4</v>
+        <v>5.3</v>
       </c>
       <c r="F20" s="21">
-        <v>2.5</v>
+        <v>4.2</v>
       </c>
       <c r="G20" s="21">
-        <v>2.1</v>
+        <v>11.1</v>
       </c>
       <c r="H20" s="21">
-        <v>18.3</v>
+        <v>5.3</v>
       </c>
       <c r="I20" s="21">
-        <v>14.5</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="22" t="s">
-        <v>6</v>
+      <c r="A21" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B21" s="21">
-        <v>32.9</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="C21" s="21">
-        <v>34.5</v>
+        <v>21.5</v>
       </c>
       <c r="D21" s="21">
-        <v>27.1</v>
+        <v>28.1</v>
       </c>
       <c r="E21" s="21">
-        <v>42</v>
+        <v>16.2</v>
       </c>
       <c r="F21" s="21">
-        <v>38.4</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G21" s="21">
-        <v>41.2</v>
+        <v>35.9</v>
       </c>
       <c r="H21" s="21">
-        <v>35.4</v>
+        <v>17.7</v>
       </c>
       <c r="I21" s="21">
-        <v>35.200000000000003</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="6" t="s">
-        <v>76</v>
+      <c r="A22" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="B22" s="21">
-        <v>69</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C22" s="21">
-        <v>66.5</v>
+        <v>8</v>
       </c>
       <c r="D22" s="21">
-        <v>62.6</v>
+        <v>10.1</v>
       </c>
       <c r="E22" s="21">
-        <v>69.8</v>
+        <v>6.4</v>
       </c>
       <c r="F22" s="21">
-        <v>68.400000000000006</v>
+        <v>13.1</v>
       </c>
       <c r="G22" s="21">
-        <v>59.9</v>
+        <v>24.3</v>
       </c>
       <c r="H22" s="21">
-        <v>68.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I22" s="21">
-        <v>62.9</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="6" t="s">
-        <v>77</v>
+      <c r="A23" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B23" s="21">
-        <v>9.5</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="C23" s="21">
-        <v>6.8</v>
+        <v>35.5</v>
       </c>
       <c r="D23" s="21">
-        <v>7.5</v>
+        <v>34.6</v>
       </c>
       <c r="E23" s="21">
-        <v>8.5</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F23" s="21">
-        <v>3</v>
+        <v>33.4</v>
       </c>
       <c r="G23" s="21">
-        <v>10.7</v>
+        <v>35.6</v>
       </c>
       <c r="H23" s="21">
-        <v>6.4</v>
+        <v>36.4</v>
       </c>
       <c r="I23" s="21">
-        <v>9.6</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="A24" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="23">
+        <v>13.8</v>
+      </c>
+      <c r="C24" s="23">
+        <v>15.5</v>
+      </c>
+      <c r="D24" s="23">
+        <v>15.8</v>
+      </c>
+      <c r="E24" s="23">
+        <v>16.7</v>
+      </c>
+      <c r="F24" s="23">
+        <v>12.6</v>
+      </c>
+      <c r="G24" s="23">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="H24" s="23">
+        <v>15.5</v>
+      </c>
+      <c r="I24" s="23">
+        <v>17.8</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="21">
-        <v>6</v>
-      </c>
-      <c r="C25" s="21">
-        <v>6.9</v>
-      </c>
-      <c r="D25" s="21">
-        <v>9.6</v>
-      </c>
-      <c r="E25" s="21">
-        <v>5.3</v>
-      </c>
-      <c r="F25" s="21">
-        <v>4.2</v>
-      </c>
-      <c r="G25" s="21">
-        <v>11.1</v>
-      </c>
-      <c r="H25" s="21">
-        <v>5.3</v>
-      </c>
-      <c r="I25" s="21">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="21">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="C26" s="21">
-        <v>21.5</v>
-      </c>
-      <c r="D26" s="21">
-        <v>28.1</v>
-      </c>
-      <c r="E26" s="21">
-        <v>16.2</v>
-      </c>
-      <c r="F26" s="21">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="G26" s="21">
-        <v>35.9</v>
-      </c>
-      <c r="H26" s="21">
-        <v>17.7</v>
-      </c>
-      <c r="I26" s="21">
-        <v>29.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="21">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C27" s="21">
-        <v>8</v>
-      </c>
-      <c r="D27" s="21">
-        <v>10.1</v>
-      </c>
-      <c r="E27" s="21">
-        <v>6.4</v>
-      </c>
-      <c r="F27" s="21">
-        <v>13.1</v>
-      </c>
-      <c r="G27" s="21">
-        <v>24.3</v>
-      </c>
-      <c r="H27" s="21">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="I27" s="21">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="21">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="C29" s="21">
-        <v>35.5</v>
-      </c>
-      <c r="D29" s="21">
-        <v>34.6</v>
-      </c>
-      <c r="E29" s="21">
-        <v>32.799999999999997</v>
-      </c>
-      <c r="F29" s="21">
-        <v>33.4</v>
-      </c>
-      <c r="G29" s="21">
-        <v>35.6</v>
-      </c>
-      <c r="H29" s="21">
-        <v>36.4</v>
-      </c>
-      <c r="I29" s="21">
-        <v>36.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="23">
-        <v>13.8</v>
-      </c>
-      <c r="C30" s="23">
-        <v>15.5</v>
-      </c>
-      <c r="D30" s="23">
-        <v>15.8</v>
-      </c>
-      <c r="E30" s="23">
-        <v>16.7</v>
-      </c>
-      <c r="F30" s="23">
-        <v>12.6</v>
-      </c>
-      <c r="G30" s="23">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="H30" s="23">
-        <v>15.5</v>
-      </c>
-      <c r="I30" s="23">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4753,10 +4677,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -4778,13 +4702,13 @@
         <v>21</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>17</v>
@@ -4793,7 +4717,7 @@
         <v>71</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -4832,788 +4756,653 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>23</v>
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="21">
+        <v>48.4</v>
+      </c>
+      <c r="C3" s="21">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="D3" s="21">
+        <v>51.3</v>
+      </c>
+      <c r="E3" s="21">
+        <v>28.1</v>
+      </c>
+      <c r="F3" s="21">
+        <v>23.3</v>
+      </c>
+      <c r="G3" s="21">
+        <v>48.3</v>
+      </c>
+      <c r="H3" s="21">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="I3" s="21">
+        <v>86.8</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B4" s="21">
-        <v>48.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C4" s="21">
-        <v>64.900000000000006</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D4" s="21">
-        <v>51.3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="21">
-        <v>28.1</v>
+        <v>1.9</v>
       </c>
       <c r="F4" s="21">
-        <v>23.3</v>
+        <v>5.2</v>
       </c>
       <c r="G4" s="21">
-        <v>48.3</v>
+        <v>8.9</v>
       </c>
       <c r="H4" s="21">
-        <v>78.099999999999994</v>
+        <v>5.3</v>
       </c>
       <c r="I4" s="21">
-        <v>86.8</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="21">
+        <v>33.4</v>
+      </c>
+      <c r="C5" s="21">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D5" s="21">
+        <v>28.3</v>
+      </c>
+      <c r="E5" s="21">
+        <v>41</v>
+      </c>
+      <c r="F5" s="21">
+        <v>43.3</v>
+      </c>
+      <c r="G5" s="21">
+        <v>37.9</v>
+      </c>
+      <c r="H5" s="21">
+        <v>34.4</v>
+      </c>
+      <c r="I5" s="21">
+        <v>31.1</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
+      <c r="A6" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B6" s="21">
+        <v>69.7</v>
+      </c>
+      <c r="C6" s="21">
+        <v>65.7</v>
+      </c>
+      <c r="D6" s="21">
+        <v>62.6</v>
+      </c>
+      <c r="E6" s="21">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="F6" s="21">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G6" s="21">
+        <v>59.6</v>
+      </c>
+      <c r="H6" s="21">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="I6" s="21">
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="21">
+        <v>1.4</v>
+      </c>
+      <c r="C7" s="21">
+        <v>1.7</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1.8</v>
+      </c>
+      <c r="E7" s="21">
+        <v>2.8</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1.6</v>
+      </c>
+      <c r="G7" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="H7" s="21">
+        <v>1.6</v>
+      </c>
+      <c r="I7" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="21">
         <v>78.900000000000006</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C8" s="21">
         <v>76.3</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D8" s="21">
         <v>62</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E8" s="21">
         <v>79.400000000000006</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F8" s="21">
         <v>90.4</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G8" s="21">
         <v>61.1</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H8" s="21">
         <v>81</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I8" s="21">
         <v>68.2</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="21">
-        <v>21.1</v>
-      </c>
-      <c r="C7" s="21">
-        <v>23.7</v>
-      </c>
-      <c r="D7" s="21">
-        <v>38</v>
-      </c>
-      <c r="E7" s="21">
-        <v>20.6</v>
-      </c>
-      <c r="F7" s="21">
-        <v>9.6</v>
-      </c>
-      <c r="G7" s="21">
-        <v>38.9</v>
-      </c>
-      <c r="H7" s="21">
-        <v>19</v>
-      </c>
-      <c r="I7" s="21">
-        <v>31.8</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>4</v>
-      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="B9" s="21">
-        <v>81.7</v>
+        <v>21.1</v>
       </c>
       <c r="C9" s="21">
-        <v>77.599999999999994</v>
+        <v>23.7</v>
       </c>
       <c r="D9" s="21">
-        <v>80.400000000000006</v>
+        <v>38</v>
       </c>
       <c r="E9" s="21">
-        <v>72.2</v>
+        <v>20.6</v>
       </c>
       <c r="F9" s="21">
-        <v>80.099999999999994</v>
+        <v>9.6</v>
       </c>
       <c r="G9" s="21">
-        <v>70.7</v>
+        <v>38.9</v>
       </c>
       <c r="H9" s="21">
-        <v>76.8</v>
+        <v>19</v>
       </c>
       <c r="I9" s="21">
-        <v>77.3</v>
-      </c>
+        <v>31.8</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B10" s="21">
-        <v>11</v>
+        <v>81.7</v>
       </c>
       <c r="C10" s="21">
-        <v>16</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="D10" s="21">
-        <v>12.9</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="E10" s="21">
-        <v>24.1</v>
+        <v>72.2</v>
       </c>
       <c r="F10" s="21">
-        <v>15.6</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="G10" s="21">
-        <v>17.100000000000001</v>
+        <v>70.7</v>
       </c>
       <c r="H10" s="21">
-        <v>16.5</v>
+        <v>76.8</v>
       </c>
       <c r="I10" s="21">
-        <v>18.2</v>
+        <v>77.3</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="B11" s="21">
-        <v>3.8</v>
+        <v>11</v>
       </c>
       <c r="C11" s="21">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D11" s="21">
-        <v>3.4</v>
+        <v>12.9</v>
       </c>
       <c r="E11" s="21">
-        <v>2.7</v>
+        <v>24.1</v>
       </c>
       <c r="F11" s="21">
-        <v>2.2999999999999998</v>
+        <v>15.6</v>
       </c>
       <c r="G11" s="21">
-        <v>9.9</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="H11" s="21">
-        <v>2.6</v>
+        <v>16.5</v>
       </c>
       <c r="I11" s="21">
-        <v>2.7</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="B12" s="21">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="C12" s="21">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="21">
+        <v>3.4</v>
+      </c>
+      <c r="E12" s="21">
+        <v>2.7</v>
+      </c>
+      <c r="F12" s="21">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E12" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1.1000000000000001</v>
-      </c>
       <c r="G12" s="21">
-        <v>0.9</v>
+        <v>9.9</v>
       </c>
       <c r="H12" s="21">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="I12" s="21">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="B13" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="D13" s="21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="H13" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="I13" s="21">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="21">
         <v>1</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C14" s="21">
         <v>0.9</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D14" s="21">
         <v>1</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E14" s="21">
         <v>0.8</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F14" s="21">
         <v>0.9</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G14" s="21">
         <v>1.4</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H14" s="21">
         <v>1</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I14" s="21">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="21">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C14" s="21">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D14" s="21">
-        <v>4</v>
-      </c>
-      <c r="E14" s="21">
-        <v>1.9</v>
-      </c>
-      <c r="F14" s="21">
-        <v>5.2</v>
-      </c>
-      <c r="G14" s="21">
-        <v>8.9</v>
-      </c>
-      <c r="H14" s="21">
-        <v>5.3</v>
-      </c>
-      <c r="I14" s="21">
-        <v>3.7</v>
-      </c>
-    </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>4</v>
+      <c r="A15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="21">
+        <v>7.7</v>
+      </c>
+      <c r="C15" s="21">
+        <v>7.3</v>
+      </c>
+      <c r="D15" s="21">
+        <v>11.7</v>
+      </c>
+      <c r="E15" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="F15" s="21">
+        <v>10.1</v>
+      </c>
+      <c r="G15" s="21">
+        <v>16.3</v>
+      </c>
+      <c r="H15" s="21">
+        <v>4.8</v>
+      </c>
+      <c r="I15" s="21">
+        <v>6.3</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="B16" s="21">
-        <v>7.7</v>
+        <v>26.8</v>
       </c>
       <c r="C16" s="21">
-        <v>7.3</v>
+        <v>27.6</v>
       </c>
       <c r="D16" s="21">
-        <v>11.7</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="E16" s="21">
-        <v>5.4</v>
+        <v>42.2</v>
       </c>
       <c r="F16" s="21">
-        <v>10.1</v>
+        <v>45.4</v>
       </c>
       <c r="G16" s="21">
-        <v>16.3</v>
+        <v>41.2</v>
       </c>
       <c r="H16" s="21">
-        <v>4.8</v>
+        <v>19.2</v>
       </c>
       <c r="I16" s="21">
-        <v>6.3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="B17" s="21">
-        <v>26.8</v>
+        <v>33.9</v>
       </c>
       <c r="C17" s="21">
-        <v>27.6</v>
+        <v>38.1</v>
       </c>
       <c r="D17" s="21">
-        <v>36.200000000000003</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="E17" s="21">
-        <v>42.2</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="F17" s="21">
-        <v>45.4</v>
+        <v>35.6</v>
       </c>
       <c r="G17" s="21">
-        <v>41.2</v>
+        <v>34</v>
       </c>
       <c r="H17" s="21">
-        <v>19.2</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="I17" s="21">
-        <v>26</v>
+        <v>35.799999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="B18" s="21">
-        <v>33.9</v>
+        <v>20</v>
       </c>
       <c r="C18" s="21">
-        <v>38.1</v>
+        <v>16.5</v>
       </c>
       <c r="D18" s="21">
-        <v>36.700000000000003</v>
+        <v>11.1</v>
       </c>
       <c r="E18" s="21">
-        <v>38.299999999999997</v>
+        <v>10.9</v>
       </c>
       <c r="F18" s="21">
-        <v>35.6</v>
+        <v>7.2</v>
       </c>
       <c r="G18" s="21">
-        <v>34</v>
+        <v>6.7</v>
       </c>
       <c r="H18" s="21">
-        <v>39.700000000000003</v>
+        <v>20.7</v>
       </c>
       <c r="I18" s="21">
-        <v>35.799999999999997</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="B19" s="21">
-        <v>20</v>
+        <v>11.6</v>
       </c>
       <c r="C19" s="21">
-        <v>16.5</v>
+        <v>10.5</v>
       </c>
       <c r="D19" s="21">
-        <v>11.1</v>
+        <v>4.2</v>
       </c>
       <c r="E19" s="21">
-        <v>10.9</v>
+        <v>3.3</v>
       </c>
       <c r="F19" s="21">
-        <v>7.2</v>
+        <v>1.8</v>
       </c>
       <c r="G19" s="21">
-        <v>6.7</v>
+        <v>1.8</v>
       </c>
       <c r="H19" s="21">
-        <v>20.7</v>
+        <v>15.5</v>
       </c>
       <c r="I19" s="21">
-        <v>20.5</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="21">
+        <v>6.9</v>
+      </c>
+      <c r="C20" s="21">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D20" s="21">
+        <v>11.6</v>
+      </c>
+      <c r="E20" s="21">
+        <v>6.9</v>
+      </c>
+      <c r="F20" s="21">
+        <v>4.2</v>
+      </c>
+      <c r="G20" s="21">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H20" s="21">
+        <v>7</v>
+      </c>
+      <c r="I20" s="21">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="21">
+        <v>21.5</v>
+      </c>
+      <c r="C21" s="21">
+        <v>25.6</v>
+      </c>
+      <c r="D21" s="21">
+        <v>31.9</v>
+      </c>
+      <c r="E21" s="21">
+        <v>19.8</v>
+      </c>
+      <c r="F21" s="21">
+        <v>18.5</v>
+      </c>
+      <c r="G21" s="21">
+        <v>42.3</v>
+      </c>
+      <c r="H21" s="21">
+        <v>22.9</v>
+      </c>
+      <c r="I21" s="21">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="21">
+        <v>11</v>
+      </c>
+      <c r="C22" s="21">
+        <v>11.2</v>
+      </c>
+      <c r="D22" s="21">
+        <v>12.6</v>
+      </c>
+      <c r="E22" s="21">
+        <v>8.9</v>
+      </c>
+      <c r="F22" s="21">
+        <v>14.5</v>
+      </c>
+      <c r="G22" s="21">
+        <v>27.9</v>
+      </c>
+      <c r="H22" s="21">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I22" s="21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="21">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="C23" s="21">
+        <v>36.5</v>
+      </c>
+      <c r="D23" s="21">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E23" s="21">
+        <v>34.4</v>
+      </c>
+      <c r="F23" s="21">
+        <v>32.1</v>
+      </c>
+      <c r="G23" s="21">
+        <v>32.4</v>
+      </c>
+      <c r="H23" s="21">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="I23" s="21">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="23">
+        <v>12.8</v>
+      </c>
+      <c r="C24" s="23">
+        <v>13.5</v>
+      </c>
+      <c r="D24" s="23">
         <v>16</v>
       </c>
-      <c r="B20" s="21">
-        <v>11.6</v>
-      </c>
-      <c r="C20" s="21">
-        <v>10.5</v>
-      </c>
-      <c r="D20" s="21">
-        <v>4.2</v>
-      </c>
-      <c r="E20" s="21">
-        <v>3.3</v>
-      </c>
-      <c r="F20" s="21">
-        <v>1.8</v>
-      </c>
-      <c r="G20" s="21">
-        <v>1.8</v>
-      </c>
-      <c r="H20" s="21">
-        <v>15.5</v>
-      </c>
-      <c r="I20" s="21">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="21">
-        <v>33.4</v>
-      </c>
-      <c r="C21" s="21">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="D21" s="21">
-        <v>28.3</v>
-      </c>
-      <c r="E21" s="21">
-        <v>41</v>
-      </c>
-      <c r="F21" s="21">
-        <v>43.3</v>
-      </c>
-      <c r="G21" s="21">
-        <v>37.9</v>
-      </c>
-      <c r="H21" s="21">
-        <v>34.4</v>
-      </c>
-      <c r="I21" s="21">
-        <v>31.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="21">
-        <v>69.7</v>
-      </c>
-      <c r="C22" s="21">
-        <v>65.7</v>
-      </c>
-      <c r="D22" s="21">
-        <v>62.6</v>
-      </c>
-      <c r="E22" s="21">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="F22" s="21">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="G22" s="21">
-        <v>59.6</v>
-      </c>
-      <c r="H22" s="21">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="I22" s="21">
-        <v>63.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="21">
-        <v>1.4</v>
-      </c>
-      <c r="C23" s="21">
-        <v>1.7</v>
-      </c>
-      <c r="D23" s="21">
-        <v>1.8</v>
-      </c>
-      <c r="E23" s="21">
-        <v>2.8</v>
-      </c>
-      <c r="F23" s="21">
-        <v>1.6</v>
-      </c>
-      <c r="G23" s="21">
-        <v>3.2</v>
-      </c>
-      <c r="H23" s="21">
-        <v>1.6</v>
-      </c>
-      <c r="I23" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="E24" s="23">
+        <v>13.1</v>
+      </c>
+      <c r="F24" s="23">
+        <v>13.8</v>
+      </c>
+      <c r="G24" s="23">
+        <v>15.6</v>
+      </c>
+      <c r="H24" s="23">
+        <v>12</v>
+      </c>
+      <c r="I24" s="23">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="21">
-        <v>6.9</v>
-      </c>
-      <c r="C25" s="21">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D25" s="21">
-        <v>11.6</v>
-      </c>
-      <c r="E25" s="21">
-        <v>6.9</v>
-      </c>
-      <c r="F25" s="21">
-        <v>4.2</v>
-      </c>
-      <c r="G25" s="21">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="H25" s="21">
-        <v>7</v>
-      </c>
-      <c r="I25" s="21">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="21">
-        <v>21.5</v>
-      </c>
-      <c r="C26" s="21">
-        <v>25.6</v>
-      </c>
-      <c r="D26" s="21">
-        <v>31.9</v>
-      </c>
-      <c r="E26" s="21">
-        <v>19.8</v>
-      </c>
-      <c r="F26" s="21">
-        <v>18.5</v>
-      </c>
-      <c r="G26" s="21">
-        <v>42.3</v>
-      </c>
-      <c r="H26" s="21">
-        <v>22.9</v>
-      </c>
-      <c r="I26" s="21">
-        <v>31.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="21">
-        <v>11</v>
-      </c>
-      <c r="C27" s="21">
-        <v>11.2</v>
-      </c>
-      <c r="D27" s="21">
-        <v>12.6</v>
-      </c>
-      <c r="E27" s="21">
-        <v>8.9</v>
-      </c>
-      <c r="F27" s="21">
-        <v>14.5</v>
-      </c>
-      <c r="G27" s="21">
-        <v>27.9</v>
-      </c>
-      <c r="H27" s="21">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="I27" s="21">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="21">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="C29" s="21">
-        <v>36.5</v>
-      </c>
-      <c r="D29" s="21">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="E29" s="21">
-        <v>34.4</v>
-      </c>
-      <c r="F29" s="21">
-        <v>32.1</v>
-      </c>
-      <c r="G29" s="21">
-        <v>32.4</v>
-      </c>
-      <c r="H29" s="21">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="I29" s="21">
-        <v>36.299999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="23">
-        <v>12.8</v>
-      </c>
-      <c r="C30" s="23">
-        <v>13.5</v>
-      </c>
-      <c r="D30" s="23">
-        <v>16</v>
-      </c>
-      <c r="E30" s="23">
-        <v>13.1</v>
-      </c>
-      <c r="F30" s="23">
-        <v>13.8</v>
-      </c>
-      <c r="G30" s="23">
-        <v>15.6</v>
-      </c>
-      <c r="H30" s="23">
-        <v>12</v>
-      </c>
-      <c r="I30" s="23">
-        <v>15.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>